<commit_message>
add solar flux and habit code
</commit_message>
<xml_diff>
--- a/data_in/column_descriptions.xlsx
+++ b/data_in/column_descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Desktop\HW_LessonsCopy\BootCampHW\ETL-Project\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Desktop\HW_LessonsCopy\BootCampHW\ETL-Project\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6EE9EC-D789-44DF-B548-12773C8EFF04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F265CBB-7F73-4398-BA5A-B8742C61A666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="3120" windowWidth="7500" windowHeight="7800" xr2:uid="{7B81DA83-8CD6-4F19-8003-3F1006B3DC54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7B81DA83-8CD6-4F19-8003-3F1006B3DC54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>pl_name</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>st_dist</t>
+  </si>
+  <si>
+    <t>pl_insol</t>
+  </si>
+  <si>
+    <t>Insolation Flux [Earth Flux]</t>
   </si>
 </sst>
 </file>
@@ -547,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FA63E9-8E7A-4946-B6DE-D40ABCAE919C}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,97 +687,105 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>